<commit_message>
kaizen añadiendo oficiales y no oficiales
</commit_message>
<xml_diff>
--- a/resources/templates/kaizen.xlsx
+++ b/resources/templates/kaizen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsanchez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5147F67-8D61-4B61-BCD9-F948B2CDDBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0EB05D-F4EB-4609-BF49-A5F9A23CE0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1B020502-AD26-4614-93AD-051854F4CBAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B020502-AD26-4614-93AD-051854F4CBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="AX ENGOMADO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Fecha de modificación</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Julios</t>
+  </si>
+  <si>
+    <t>Oficiales</t>
+  </si>
+  <si>
+    <t>No. Oficiales</t>
   </si>
 </sst>
 </file>
@@ -512,15 +518,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0D240B-78E4-4D73-BDA9-E01A9589C2F9}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,8 +572,14 @@
       <c r="O1" t="s">
         <v>26</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44948</v>
       </c>
@@ -613,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2A6F55-97E7-4164-BE88-64A912EB3AA8}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +636,7 @@
     <col min="10" max="10" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -664,8 +676,14 @@
       <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>46011</v>
       </c>

</xml_diff>